<commit_message>
fix regex on unicode
</commit_message>
<xml_diff>
--- a/public/samples/eoc.xlsx
+++ b/public/samples/eoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radin/workspaces/projects/mobiles/eoc/eoc-web/public/sops document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radin/workspaces/projects/mobiles/eoc/eoc-web/public/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC629639-321A-6544-B1F1-03AB94EEE344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72394863-C152-5840-8F33-C0D74357C3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{358E6273-6845-9640-97D8-3CF1984D4745}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="22160" windowHeight="20540" activeTab="1" xr2:uid="{358E6273-6845-9640-97D8-3CF1984D4745}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="120">
   <si>
     <t>parent</t>
   </si>
@@ -1609,13 +1609,214 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>ADHD</t>
+  </si>
+  <si>
+    <t>Predominantly Inattentive Presentation</t>
+  </si>
+  <si>
+    <t>Predominantly Hyperactive-Impulsive Presentation</t>
+  </si>
+  <si>
+    <t>Combined Presentation</t>
+  </si>
+  <si>
+    <t>It is hard for the individual to organize or finish a task, to pay attention to details, or to follow instructions or conversations. The person is easily distracted or forgets details of daily routines.</t>
+  </si>
+  <si>
+    <t>The person fidgets and talks a lot. It is hard to sit still for long (e.g., for a meal or while doing homework)</t>
+  </si>
+  <si>
+    <t>Symptoms of the above two types are equally present in the person</t>
+  </si>
+  <si>
+    <t>Combined Presentation.pdf</t>
+  </si>
+  <si>
+    <t>Predominantly Hyperactive.pdf</t>
+  </si>
+  <si>
+    <t>Predominantly Inattentive Presentation.pdf</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Type 1 diabetes</t>
+  </si>
+  <si>
+    <t>type 2 diabetes</t>
+  </si>
+  <si>
+    <t>Gestational diabetes</t>
+  </si>
+  <si>
+    <t>Type 1 diabetes.pdf</t>
+  </si>
+  <si>
+    <t>type 2 diabetes.pdf</t>
+  </si>
+  <si>
+    <t>Gestational diabetes.pdf</t>
+  </si>
+  <si>
+    <t>Type 1 diabetes (previously called insulin-dependent or juvenile diabetes) is usually diagnosed in children, teens, and young adults, but it can develop at any age.</t>
+  </si>
+  <si>
+    <t>your body doesn’t use insulin well and can’t keep blood sugar at normal levels. About 90% of people with diabetes have type 2</t>
+  </si>
+  <si>
+    <t>develops in pregnant women who have never had diabetes</t>
+  </si>
+  <si>
+    <t>Seasonal Flu</t>
+  </si>
+  <si>
+    <t>Get Vaccinated</t>
+  </si>
+  <si>
+    <t>Preventive Steps</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Who should get</t>
+  </si>
+  <si>
+    <t>Who Should Not</t>
+  </si>
+  <si>
+    <t>Special Consideration</t>
+  </si>
+  <si>
+    <t>When should get</t>
+  </si>
+  <si>
+    <t>Avoid close contact</t>
+  </si>
+  <si>
+    <t>Stay home when you are sick</t>
+  </si>
+  <si>
+    <t>Cover your mouth and nose</t>
+  </si>
+  <si>
+    <t>Clean your hands</t>
+  </si>
+  <si>
+    <t>Handwashing: Clean Hands Save Lives</t>
+  </si>
+  <si>
+    <r>
+      <t>Handwashing can help prevent illness.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="17"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>It involves five simple and effective steps (Wet, Lather, Scrub, Rinse, Dry) you can take to reduce the spread of diarrheal and respiratory illness so you can stay healthy</t>
+    </r>
+  </si>
+  <si>
+    <t>Clean your hands.pdf</t>
+  </si>
+  <si>
+    <t>ជំងឺមហារីក</t>
+  </si>
+  <si>
+    <t>ការគ្រប់គ្រងការចង្អោលើអ្នកជំងឺមហារីក</t>
+  </si>
+  <si>
+    <t>ការចង្អោដែលកើតឡើងលើអ្នកជំងឺមហារីកប្រហែលជាបង្កឡើងដោយបាក់តេរីក្នុងអាហារ រហូតដល់ការប្រើថ្នាំមហារីក</t>
+  </si>
+  <si>
+    <t>ជំងឺមហារីក.pdf</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>Ischemic stroke.</t>
+  </si>
+  <si>
+    <t>Hemorrhagic stroke.</t>
+  </si>
+  <si>
+    <t>Transient ischemic attack (a warning or “mini-stroke”).</t>
+  </si>
+  <si>
+    <t>Ischemic Stroke</t>
+  </si>
+  <si>
+    <t>Ischemic Stroke.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t>Most strokes (87%) are ischemic strokes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t> An ischemic stroke happens when blood flow through the artery that supplies oxygen-rich blood to the brain becomes blocked.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hemorrhagic Stroke</t>
+  </si>
+  <si>
+    <t>Hemorrhagic Stroke.pdf</t>
+  </si>
+  <si>
+    <t>A hemorrhagic stroke happens when an artery in the brain leaks blood or ruptures (breaks open). The leaked blood puts too much pressure on brain cells, which damages them.</t>
+  </si>
+  <si>
+    <t>Transient Ischemic Attack (TIA)</t>
+  </si>
+  <si>
+    <t>Transient Ischemic Attack.pdf</t>
+  </si>
+  <si>
+    <t>A transient ischemic attack (TIA) is sometimes called a “mini-stroke.” It is different from the major types of stroke because blood flow to </t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1684,11 +1885,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <i/>
-      <sz val="12"/>
+      <sz val="17"/>
       <color rgb="FF000000"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7.8"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1711,7 +1925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1725,7 +1939,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2040,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB3E9B3-C53D-524E-A74C-3E7A761AE0C5}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2074,11 +2287,200 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2088,16 +2490,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E5C96A-7EF2-0541-8248-20B51F12651F}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="69.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -2345,7 +2747,7 @@
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C15" t="s">
@@ -2362,7 +2764,7 @@
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C16" t="s">
@@ -2375,41 +2777,228 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="22" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" ht="22" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A23" r:id="rId1" display="https://www.cdc.gov/handwashing/index.html" xr:uid="{72E77377-B395-E949-9614-A364F45DB977}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix wrong category name
</commit_message>
<xml_diff>
--- a/public/samples/eoc.xlsx
+++ b/public/samples/eoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radin/workspaces/projects/mobiles/eoc/eoc-web/public/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8691B70C-9457-1442-928D-5B209716599F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6427FF38-509C-4F4B-860F-E91464C6B2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="22160" windowHeight="20540" activeTab="1" xr2:uid="{358E6273-6845-9640-97D8-3CF1984D4745}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="22160" windowHeight="20540" xr2:uid="{358E6273-6845-9640-97D8-3CF1984D4745}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -2264,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB3E9B3-C53D-524E-A74C-3E7A761AE0C5}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2499,10 +2499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E5C96A-7EF2-0541-8248-20B51F12651F}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2939,8 +2939,8 @@
       <c r="D25" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>110</v>
+      <c r="E25" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -2957,8 +2957,8 @@
       <c r="D26" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>113</v>
+      <c r="E26" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -2975,8 +2975,8 @@
       <c r="D27" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>116</v>
+      <c r="E27" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="F27" s="8"/>
     </row>
@@ -3006,14 +3006,6 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A23" r:id="rId1" display="https://www.cdc.gov/handwashing/index.html" xr:uid="{72E77377-B395-E949-9614-A364F45DB977}"/>

</xml_diff>